<commit_message>
Student entry using excel
The module to receive student data using excel done
</commit_message>
<xml_diff>
--- a/admin/admin/assets/files/default files/students_template.xlsx
+++ b/admin/admin/assets/files/default files/students_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\shsdesk\admin\admin\assets\files\default files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B54AA76-5D9F-41F0-891B-3A5098940029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F302932-C921-4F0B-97BE-D033FABA8A4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F3A1DC9C-76C1-4FF3-B3A0-7AC3F1B45465}"/>
+    <workbookView xWindow="9660" yWindow="1176" windowWidth="12720" windowHeight="8940" xr2:uid="{F3A1DC9C-76C1-4FF3-B3A0-7AC3F1B45465}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Index Number</t>
   </si>
@@ -52,9 +52,6 @@
     <t>House</t>
   </si>
   <si>
-    <t>Guardian Contact</t>
-  </si>
-  <si>
     <t>000000001</t>
   </si>
   <si>
@@ -70,9 +67,6 @@
     <t>House Name</t>
   </si>
   <si>
-    <t>0123456789</t>
-  </si>
-  <si>
     <t>Year</t>
   </si>
   <si>
@@ -86,6 +80,33 @@
   </si>
   <si>
     <t>Boarder</t>
+  </si>
+  <si>
+    <t>Class Name</t>
+  </si>
+  <si>
+    <t>Science 1</t>
+  </si>
+  <si>
+    <t>Amega</t>
+  </si>
+  <si>
+    <t>Aisha</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>House three</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Visual Arts</t>
+  </si>
+  <si>
+    <t>Vis 2</t>
   </si>
 </sst>
 </file>
@@ -121,10 +142,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E33E52AF-89E8-44BF-BE29-C475CD22548C}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -451,10 +471,11 @@
     <col min="2" max="2" width="8.88671875" style="1"/>
     <col min="3" max="3" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.88671875" style="1"/>
-    <col min="5" max="5" width="8.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" customWidth="1"/>
     <col min="6" max="6" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -470,49 +491,75 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>12</v>
+      <c r="E1" t="s">
+        <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2">
-        <v>2</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="G2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>11</v>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>